<commit_message>
Undergo Optimization -- topological similarity
</commit_message>
<xml_diff>
--- a/src/test/java/resources/AlgTest/HGA/graph1.xlsx
+++ b/src/test/java/resources/AlgTest/HGA/graph1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Algorithms\src\test\java\resources\AlgTest\HGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA09E5B3-F1E2-4059-B40E-333DC84619A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9055690A-FC83-4096-9918-6914FD9859D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6504" yWindow="4272" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="3540" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>A</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Target</t>
   </si>
 </sst>
 </file>
@@ -372,20 +378,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -425,15 +431,15 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -441,7 +447,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -449,7 +455,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -457,15 +463,15 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -473,7 +479,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -481,15 +487,15 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -497,6 +503,14 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>